<commit_message>
update code for fix bugs
</commit_message>
<xml_diff>
--- a/metadata-file-2024.xlsx
+++ b/metadata-file-2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U324"/>
+  <dimension ref="A1:V324"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,6 +539,11 @@
           <t>date</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>session_name_as_folder_name</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -636,6 +641,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Flow, Topology, and Uncertainty</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -737,6 +747,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Look, Learn, Language Models</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -834,6 +849,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Where the Networks Are</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -931,6 +951,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Human and Machine Visualization Literacy</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1012,6 +1037,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>Test of Time Awards</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1095,6 +1125,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>IEEE VIS Capstone and Closing</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1174,6 +1209,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>IEEE VIS Capstone and Closing</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1257,6 +1297,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>IEEE VIS Capstone and Closing</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1342,11 +1387,16 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>Progressive Data Analysis and Visualization (PDAV) Workshop</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Uncertainty Visualization-Applications, Techniques, Software, and Decision Frameworks</t>
+          <t>Uncertainty Visualization: Applications, Techniques, Software, and Decision Frameworks</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1427,6 +1477,11 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Uncertainty Visualization-Applications, Techniques, Software, and Decision Frameworks</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1512,6 +1567,11 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>Visualization for Climate Action and Sustainability</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1597,11 +1657,16 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>VisInPractice</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BELIV-evaluation and BEyond - methodoLogIcal approaches for Visualization</t>
+          <t>BELIV: evaluation and BEyond - methodoLogIcal approaches for Visualization</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1682,6 +1747,11 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>BELIV-evaluation and BEyond - methodoLogIcal approaches for Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1767,11 +1837,16 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>SciVis Contest</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>LLM4Vis-Large Language Models for Information Visualization</t>
+          <t>LLM4Vis: Large Language Models for Information Visualization</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1852,11 +1927,16 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>LLM4Vis-Large Language Models for Information Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>NLVIZ Workshop-Exploring Research Opportunities for Natural Language, Text, and Data Visualization</t>
+          <t>NLVIZ Workshop: Exploring Research Opportunities for Natural Language, Text, and Data Visualization</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1937,11 +2017,16 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>NLVIZ Workshop-Exploring Research Opportunities for Natural Language, Text, and Data Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>EnergyVis 2024-4th Workshop on Energy Data Visualization</t>
+          <t>EnergyVis 2024: 4th Workshop on Energy Data Visualization</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2022,11 +2107,16 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>EnergyVis 2024-4th Workshop on Energy Data Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>VISions of the Future-Workshop on Sustainable Practices within Visualization and Physicalisation</t>
+          <t>VISions of the Future: Workshop on Sustainable Practices within Visualization and Physicalisation</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2107,11 +2197,16 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>VISions of the Future-Workshop on Sustainable Practices within Visualization and Physicalisation</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TopoInVis-Workshop on Topological Data Analysis and Visualization</t>
+          <t>TopoInVis: Workshop on Topological Data Analysis and Visualization</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2192,11 +2287,16 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>TopoInVis-Workshop on Topological Data Analysis and Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BELIV-evaluation and BEyond - methodoLogIcal approaches for Visualization</t>
+          <t>BELIV: evaluation and BEyond - methodoLogIcal approaches for Visualization</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2277,6 +2377,11 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>BELIV-evaluation and BEyond - methodoLogIcal approaches for Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2362,11 +2467,16 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>Preparing, Conducting, and Analyzing Participatory Design Sessions for Information Visualizations</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Enabling Scientific Discovery-A Tutorial for Harnessing the Power of the National Science Data Fabric for Large-Scale Data Analysis</t>
+          <t>Enabling Scientific Discovery: A Tutorial for Harnessing the Power of the National Science Data Fabric for Large-Scale Data Analysis</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2447,11 +2557,16 @@
           <t>Monday (Oct 14)</t>
         </is>
       </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>Enabling Scientific Discovery-A Tutorial for Harnessing the Power of the National Science Data Fabric for Large-Scale Data Analysis</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>EduVis-2nd IEEE VIS Workshop on Visualization Education, Literacy, and Activities</t>
+          <t>EduVis: 2nd IEEE VIS Workshop on Visualization Education, Literacy, and Activities</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2532,6 +2647,11 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>EduVis-2nd IEEE VIS Workshop on Visualization Education, Literacy, and Activities</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2617,11 +2737,16 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>1st Workshop on Accessible Data Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>First-Person Visualizations for Outdoor Physical Activities-Challenges and Opportunities</t>
+          <t>First-Person Visualizations for Outdoor Physical Activities: Challenges and Opportunities</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2702,11 +2827,16 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>First-Person Visualizations for Outdoor Physical Activities-Challenges and Opportunities</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>VISxAI-7th Workshop on Visualization for AI Explainability</t>
+          <t>VISxAI: 7th Workshop on Visualization for AI Explainability</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2787,6 +2917,11 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>VISxAI-7th Workshop on Visualization for AI Explainability</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2872,6 +3007,11 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>VAST Challenge</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2957,6 +3097,11 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>Visualization Analysis and Design</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3042,11 +3187,16 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V30" t="inlineStr">
+        <is>
+          <t>Developing Immersive and Collaborative Visualizations with Web Technologies</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>EduVis-2nd IEEE VIS Workshop on Visualization Education, Literacy, and Activities</t>
+          <t>EduVis: 2nd IEEE VIS Workshop on Visualization Education, Literacy, and Activities</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3127,6 +3277,11 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V31" t="inlineStr">
+        <is>
+          <t>EduVis-2nd IEEE VIS Workshop on Visualization Education, Literacy, and Activities</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3212,11 +3367,16 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>Workshop on Data Storytelling in an Era of Generative AI</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>LDAV-14th IEEE Symposium on Large Data Analysis and Visualization</t>
+          <t>LDAV: 14th IEEE Symposium on Large Data Analysis and Visualization</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3297,11 +3457,16 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>LDAV-14th IEEE Symposium on Large Data Analysis and Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>VDS-Visualization in Data Science Symposium</t>
+          <t>VDS: Visualization in Data Science Symposium</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3382,6 +3547,11 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>VDS-Visualization in Data Science Symposium</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3467,6 +3637,11 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V35" t="inlineStr">
+        <is>
+          <t>Bio+Med+Vis Workshop</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3552,6 +3727,11 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V36" t="inlineStr">
+        <is>
+          <t>Generating Color Schemes for your Data Visualizations</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3637,6 +3817,11 @@
           <t>Sunday (Oct 13)</t>
         </is>
       </c>
+      <c r="V37" t="inlineStr">
+        <is>
+          <t>Running Online User Studies with the reVISit Framework</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3722,11 +3907,16 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V38" t="inlineStr">
+        <is>
+          <t>IEEE VIS 2025 Kickoff</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Panel-Human-Centered Computing Research in South America-Status Quo, Opportunities, and Challenges</t>
+          <t>Panel: Human-Centered Computing Research in South America: Status Quo, Opportunities, and Challenges</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3807,6 +3997,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V39" t="inlineStr">
+        <is>
+          <t>Panel-Human-Centered Computing Research in South America-Status Quo, Opportunities, and Challenges</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3904,6 +4099,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V40" t="inlineStr">
+        <is>
+          <t>Embeddings and Document Spatialization</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4001,6 +4201,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>Visualization Recommendation</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4102,11 +4307,16 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V42" t="inlineStr">
+        <is>
+          <t>Model-checking and Validation</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Short Papers-Perception and Representation</t>
+          <t>Short Papers: Perception and Representation</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4197,13 +4407,18 @@
       <c r="U43" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V43" t="inlineStr">
+        <is>
+          <t>Short Papers-Perception and Representation</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Panel-(Yet Another) Evaluation Needed? A Panel Discussion on Evaluation Trends in Visualization</t>
+          <t>Panel: (Yet Another) Evaluation Needed? A Panel Discussion on Evaluation Trends in Visualization</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -4284,6 +4499,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V44" t="inlineStr">
+        <is>
+          <t>Panel-(Yet Another) Evaluation Needed? A Panel Discussion on Evaluation Trends in Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4365,11 +4585,16 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t>VISAP Pictorials</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Applications-Sports. Games, and Finance</t>
+          <t>Applications: Sports. Games, and Finance</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -4460,6 +4685,11 @@
       <c r="U46" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>Applications-Sports. Games, and Finance</t>
         </is>
       </c>
     </row>
@@ -4559,11 +4789,16 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>Topological Data Analysis</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Visual Design-Sketching and Labeling</t>
+          <t>Visual Design: Sketching and Labeling</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4654,13 +4889,18 @@
       <c r="U48" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V48" t="inlineStr">
+        <is>
+          <t>Visual Design-Sketching and Labeling</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Short Papers-Text and Multimedia</t>
+          <t>Short Papers: Text and Multimedia</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4751,13 +4991,18 @@
       <c r="U49" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V49" t="inlineStr">
+        <is>
+          <t>Short Papers-Text and Multimedia</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Panel-Vogue or Visionary? Current Challenges and Future Opportunities in Situated Visualizations</t>
+          <t>Panel: Vogue or Visionary? Current Challenges and Future Opportunities in Situated Visualizations</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4838,6 +5083,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V50" t="inlineStr">
+        <is>
+          <t>Panel-Vogue or Visionary? Current Challenges and Future Opportunities in Situated Visualizations</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4935,6 +5185,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V51" t="inlineStr">
+        <is>
+          <t>The Toolboxes of Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -5032,6 +5287,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V52" t="inlineStr">
+        <is>
+          <t>Once Upon a Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -5129,11 +5389,16 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V53" t="inlineStr">
+        <is>
+          <t>Visualization Design Methods</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Short Papers-Analytics and Applications</t>
+          <t>Short Papers: Analytics and Applications</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -5224,13 +5489,18 @@
       <c r="U54" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V54" t="inlineStr">
+        <is>
+          <t>Short Papers-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
+          <t>CG&amp;A: Systems, Theory, and Evaluations</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -5321,13 +5591,18 @@
       <c r="U55" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V55" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Panel-Dear Younger Me-A Dialog About Professional Development Beyond The Initial Career Phases</t>
+          <t>Panel: Dear Younger Me: A Dialog About Professional Development Beyond The Initial Career Phases</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -5408,11 +5683,16 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V56" t="inlineStr">
+        <is>
+          <t>Panel-Dear Younger Me-A Dialog About Professional Development Beyond The Initial Career Phases</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Applications-Industry, Computing, and Medicine</t>
+          <t>Applications: Industry, Computing, and Medicine</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -5503,6 +5783,11 @@
       <c r="U57" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V57" t="inlineStr">
+        <is>
+          <t>Applications-Industry, Computing, and Medicine</t>
         </is>
       </c>
     </row>
@@ -5602,6 +5887,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V58" t="inlineStr">
+        <is>
+          <t>Motion and Animated Notions</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -5699,6 +5989,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V59" t="inlineStr">
+        <is>
+          <t>Journalism and Public Policy</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -5796,11 +6091,16 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t>Accessibility and Touch</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Short Papers-AI and LLM</t>
+          <t>Short Papers: AI and LLM</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5891,6 +6191,11 @@
       <c r="U61" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V61" t="inlineStr">
+        <is>
+          <t>Short Papers-AI and LLM</t>
         </is>
       </c>
     </row>
@@ -5972,6 +6277,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t>VIS Governance</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -6051,6 +6361,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t>VIS Governance</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -6134,6 +6449,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V64" t="inlineStr">
+        <is>
+          <t>Opening Session</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -6217,6 +6537,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V65" t="inlineStr">
+        <is>
+          <t>Opening Session</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -6296,6 +6621,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V66" t="inlineStr">
+        <is>
+          <t>VGTC Awards &amp; Best Short Papers</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -6387,6 +6717,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>VGTC Awards &amp; Best Short Papers</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -6488,6 +6823,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V68" t="inlineStr">
+        <is>
+          <t>VGTC Awards &amp; Best Short Papers</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -6589,6 +6929,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V69" t="inlineStr">
+        <is>
+          <t>VGTC Awards &amp; Best Short Papers</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -6680,6 +7025,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V70" t="inlineStr">
+        <is>
+          <t>Best Full Papers</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -6781,6 +7131,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V71" t="inlineStr">
+        <is>
+          <t>Best Full Papers</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -6882,6 +7237,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V72" t="inlineStr">
+        <is>
+          <t>Best Full Papers</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -6983,6 +7343,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V73" t="inlineStr">
+        <is>
+          <t>Best Full Papers</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -7084,6 +7449,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V74" t="inlineStr">
+        <is>
+          <t>Best Full Papers</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -7185,6 +7555,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V75" t="inlineStr">
+        <is>
+          <t>Best Full Papers</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -7268,6 +7643,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V76" t="inlineStr">
+        <is>
+          <t>VISAP Keynote</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -7347,6 +7727,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V77" t="inlineStr">
+        <is>
+          <t>VISAP Opening Reception</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -7428,11 +7813,16 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V78" t="inlineStr">
+        <is>
+          <t>Posters</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Application Spotlight-IEEE VIS Demos Session</t>
+          <t>Application Spotlight: IEEE VIS Demos Session</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -7513,6 +7903,11 @@
           <t>Tuesday (Oct 15)</t>
         </is>
       </c>
+      <c r="V79" t="inlineStr">
+        <is>
+          <t>Application Spotlight-IEEE VIS Demos Session</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -7594,11 +7989,16 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V80" t="inlineStr">
+        <is>
+          <t>IEEE VIS Town Hall</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Panel-VIS Conference Futures-Community Opinions on Recent Experiences, Challenges, and Opportunities for Hybrid Event Formats</t>
+          <t>Panel: VIS Conference Futures: Community Opinions on Recent Experiences, Challenges, and Opportunities for Hybrid Event Formats</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -7679,11 +8079,16 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V81" t="inlineStr">
+        <is>
+          <t>Panel-VIS Conference Futures-Community Opinions on Recent Experiences, Challenges, and Opportunities for Hybrid Event Formats</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Panel-What Do Visualization Art Projects Bring to the VIS Community?</t>
+          <t>Panel: What Do Visualization Art Projects Bring to the VIS Community?</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -7764,6 +8169,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V82" t="inlineStr">
+        <is>
+          <t>Panel-What Do Visualization Art Projects Bring to the VIS Community?</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -7861,6 +8271,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V83" t="inlineStr">
+        <is>
+          <t>Text, Annotation, and Metaphor</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -7958,6 +8373,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V84" t="inlineStr">
+        <is>
+          <t>Immersive Visualization and Visual Analytics</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -8055,11 +8475,16 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V85" t="inlineStr">
+        <is>
+          <t>Machine Learning for Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Virtual-VIS from around the world</t>
+          <t>Virtual: VIS from around the world</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -8150,13 +8575,18 @@
       <c r="U86" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V86" t="inlineStr">
+        <is>
+          <t>Virtual-VIS from around the world</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
+          <t>Short Papers: Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -8247,6 +8677,11 @@
       <c r="U87" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V87" t="inlineStr">
+        <is>
+          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
     </row>
@@ -8330,6 +8765,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V88" t="inlineStr">
+        <is>
+          <t>VISAP Papers and Artist Talks</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -8427,6 +8867,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V89" t="inlineStr">
+        <is>
+          <t>Dimensionality Reduction</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -8524,6 +8969,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V90" t="inlineStr">
+        <is>
+          <t>Urban Planning, Construction, and Disaster Management</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -8621,6 +9071,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V91" t="inlineStr">
+        <is>
+          <t>Biological Data Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -8718,6 +9173,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V92" t="inlineStr">
+        <is>
+          <t>Judgment and Decision-making</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -8815,11 +9275,16 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V93" t="inlineStr">
+        <is>
+          <t>Time and Sequences</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Virtual-Virtual VISits</t>
+          <t>Virtual: Virtual VISits</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -8910,13 +9375,18 @@
       <c r="U94" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V94" t="inlineStr">
+        <is>
+          <t>Virtual-Virtual VISits</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Panel-20 Years of Visual Analytics</t>
+          <t>Panel: 20 Years of Visual Analytics</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -8997,6 +9467,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V95" t="inlineStr">
+        <is>
+          <t>Panel-20 Years of Visual Analytics</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -9098,6 +9573,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V96" t="inlineStr">
+        <is>
+          <t>Natural Language and Multimodal Interaction</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -9195,6 +9675,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V97" t="inlineStr">
+        <is>
+          <t>Collaboration and Communication</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -9292,11 +9777,16 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V98" t="inlineStr">
+        <is>
+          <t>Perception and Cognition</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Short Papers-Scientific and Immersive Visualization</t>
+          <t>Short Papers: Scientific and Immersive Visualization</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -9387,13 +9877,18 @@
       <c r="U99" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V99" t="inlineStr">
+        <is>
+          <t>Short Papers-Scientific and Immersive Visualization</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>CG&amp;A-Analytics and Applications</t>
+          <t>CG&amp;A: Analytics and Applications</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -9484,13 +9979,18 @@
       <c r="U100" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V100" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Application Spotlight-Visualization within the Department of Energy</t>
+          <t>Application Spotlight: Visualization within the Department of Energy</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -9571,11 +10071,16 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V101" t="inlineStr">
+        <is>
+          <t>Application Spotlight-Visualization within the Department of Energy</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Panel-Past, Present, and Future of Data Storytelling</t>
+          <t>Panel: Past, Present, and Future of Data Storytelling</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -9656,6 +10161,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V102" t="inlineStr">
+        <is>
+          <t>Panel-Past, Present, and Future of Data Storytelling</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -9753,6 +10263,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V103" t="inlineStr">
+        <is>
+          <t>Designing Palettes and Encodings</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -9850,6 +10365,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V104" t="inlineStr">
+        <is>
+          <t>Of Nodes and Networks</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -9947,11 +10467,16 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V105" t="inlineStr">
+        <is>
+          <t>Scripts, Notebooks, and Provenance</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Short Papers- System design</t>
+          <t>Short Papers:  System design</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -10042,13 +10567,18 @@
       <c r="U106" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V106" t="inlineStr">
+        <is>
+          <t>Short Papers- System design</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Applications-Sports. Games, and Finance</t>
+          <t>Applications: Sports. Games, and Finance</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -10139,13 +10669,18 @@
       <c r="U107" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V107" t="inlineStr">
+        <is>
+          <t>Applications-Sports. Games, and Finance</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Applications-Sports. Games, and Finance</t>
+          <t>Applications: Sports. Games, and Finance</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -10236,13 +10771,18 @@
       <c r="U108" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V108" t="inlineStr">
+        <is>
+          <t>Applications-Sports. Games, and Finance</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Applications-Sports. Games, and Finance</t>
+          <t>Applications: Sports. Games, and Finance</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -10333,13 +10873,18 @@
       <c r="U109" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V109" t="inlineStr">
+        <is>
+          <t>Applications-Sports. Games, and Finance</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Applications-Sports. Games, and Finance</t>
+          <t>Applications: Sports. Games, and Finance</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -10430,13 +10975,18 @@
       <c r="U110" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V110" t="inlineStr">
+        <is>
+          <t>Applications-Sports. Games, and Finance</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Applications-Sports. Games, and Finance</t>
+          <t>Applications: Sports. Games, and Finance</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -10527,13 +11077,18 @@
       <c r="U111" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V111" t="inlineStr">
+        <is>
+          <t>Applications-Sports. Games, and Finance</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Applications-Industry, Computing, and Medicine</t>
+          <t>Applications: Industry, Computing, and Medicine</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -10624,13 +11179,18 @@
       <c r="U112" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V112" t="inlineStr">
+        <is>
+          <t>Applications-Industry, Computing, and Medicine</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Applications-Industry, Computing, and Medicine</t>
+          <t>Applications: Industry, Computing, and Medicine</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -10721,13 +11281,18 @@
       <c r="U113" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V113" t="inlineStr">
+        <is>
+          <t>Applications-Industry, Computing, and Medicine</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Applications-Industry, Computing, and Medicine</t>
+          <t>Applications: Industry, Computing, and Medicine</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -10818,13 +11383,18 @@
       <c r="U114" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V114" t="inlineStr">
+        <is>
+          <t>Applications-Industry, Computing, and Medicine</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Applications-Industry, Computing, and Medicine</t>
+          <t>Applications: Industry, Computing, and Medicine</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -10915,13 +11485,18 @@
       <c r="U115" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V115" t="inlineStr">
+        <is>
+          <t>Applications-Industry, Computing, and Medicine</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Applications-Industry, Computing, and Medicine</t>
+          <t>Applications: Industry, Computing, and Medicine</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -11012,6 +11587,11 @@
       <c r="U116" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V116" t="inlineStr">
+        <is>
+          <t>Applications-Industry, Computing, and Medicine</t>
         </is>
       </c>
     </row>
@@ -11111,6 +11691,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V117" t="inlineStr">
+        <is>
+          <t>Flow, Topology, and Uncertainty</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -11208,6 +11793,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V118" t="inlineStr">
+        <is>
+          <t>Flow, Topology, and Uncertainty</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -11305,6 +11895,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V119" t="inlineStr">
+        <is>
+          <t>Flow, Topology, and Uncertainty</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -11402,6 +11997,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V120" t="inlineStr">
+        <is>
+          <t>Flow, Topology, and Uncertainty</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -11499,6 +12099,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V121" t="inlineStr">
+        <is>
+          <t>Flow, Topology, and Uncertainty</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -11596,6 +12201,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V122" t="inlineStr">
+        <is>
+          <t>The Toolboxes of Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -11693,6 +12303,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V123" t="inlineStr">
+        <is>
+          <t>The Toolboxes of Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -11790,6 +12405,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V124" t="inlineStr">
+        <is>
+          <t>The Toolboxes of Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -11887,6 +12507,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V125" t="inlineStr">
+        <is>
+          <t>The Toolboxes of Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -11984,6 +12609,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V126" t="inlineStr">
+        <is>
+          <t>The Toolboxes of Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -12081,6 +12711,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V127" t="inlineStr">
+        <is>
+          <t>Topological Data Analysis</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -12178,6 +12813,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V128" t="inlineStr">
+        <is>
+          <t>Topological Data Analysis</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -12275,6 +12915,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V129" t="inlineStr">
+        <is>
+          <t>Topological Data Analysis</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -12372,6 +13017,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V130" t="inlineStr">
+        <is>
+          <t>Topological Data Analysis</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -12469,6 +13119,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V131" t="inlineStr">
+        <is>
+          <t>Topological Data Analysis</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -12566,6 +13221,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V132" t="inlineStr">
+        <is>
+          <t>Motion and Animated Notions</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -12663,6 +13323,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V133" t="inlineStr">
+        <is>
+          <t>Motion and Animated Notions</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -12760,6 +13425,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V134" t="inlineStr">
+        <is>
+          <t>Motion and Animated Notions</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -12857,6 +13527,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V135" t="inlineStr">
+        <is>
+          <t>Motion and Animated Notions</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -12954,6 +13629,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V136" t="inlineStr">
+        <is>
+          <t>Motion and Animated Notions</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -13051,6 +13731,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V137" t="inlineStr">
+        <is>
+          <t>Dimensionality Reduction</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -13148,6 +13833,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V138" t="inlineStr">
+        <is>
+          <t>Dimensionality Reduction</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -13245,6 +13935,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V139" t="inlineStr">
+        <is>
+          <t>Dimensionality Reduction</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -13342,6 +14037,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V140" t="inlineStr">
+        <is>
+          <t>Dimensionality Reduction</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -13439,6 +14139,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V141" t="inlineStr">
+        <is>
+          <t>Dimensionality Reduction</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -13536,6 +14241,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V142" t="inlineStr">
+        <is>
+          <t>Urban Planning, Construction, and Disaster Management</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -13633,6 +14343,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V143" t="inlineStr">
+        <is>
+          <t>Urban Planning, Construction, and Disaster Management</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -13730,6 +14445,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V144" t="inlineStr">
+        <is>
+          <t>Urban Planning, Construction, and Disaster Management</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -13827,6 +14547,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V145" t="inlineStr">
+        <is>
+          <t>Urban Planning, Construction, and Disaster Management</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -13924,6 +14649,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V146" t="inlineStr">
+        <is>
+          <t>Urban Planning, Construction, and Disaster Management</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -14021,6 +14751,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V147" t="inlineStr">
+        <is>
+          <t>Embeddings and Document Spatialization</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -14118,6 +14853,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V148" t="inlineStr">
+        <is>
+          <t>Embeddings and Document Spatialization</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -14215,6 +14955,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V149" t="inlineStr">
+        <is>
+          <t>Embeddings and Document Spatialization</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -14312,6 +15057,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V150" t="inlineStr">
+        <is>
+          <t>Embeddings and Document Spatialization</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -14409,6 +15159,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V151" t="inlineStr">
+        <is>
+          <t>Embeddings and Document Spatialization</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -14506,6 +15261,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V152" t="inlineStr">
+        <is>
+          <t>Designing Palettes and Encodings</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -14607,6 +15367,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V153" t="inlineStr">
+        <is>
+          <t>Designing Palettes and Encodings</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -14704,6 +15469,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V154" t="inlineStr">
+        <is>
+          <t>Designing Palettes and Encodings</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -14801,6 +15571,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V155" t="inlineStr">
+        <is>
+          <t>Designing Palettes and Encodings</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -14898,6 +15673,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V156" t="inlineStr">
+        <is>
+          <t>Designing Palettes and Encodings</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -14995,6 +15775,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V157" t="inlineStr">
+        <is>
+          <t>Text, Annotation, and Metaphor</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -15092,6 +15877,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V158" t="inlineStr">
+        <is>
+          <t>Text, Annotation, and Metaphor</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -15193,6 +15983,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V159" t="inlineStr">
+        <is>
+          <t>Text, Annotation, and Metaphor</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -15294,6 +16089,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V160" t="inlineStr">
+        <is>
+          <t>Text, Annotation, and Metaphor</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -15395,6 +16195,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V161" t="inlineStr">
+        <is>
+          <t>Text, Annotation, and Metaphor</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -15492,6 +16297,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V162" t="inlineStr">
+        <is>
+          <t>Journalism and Public Policy</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -15589,6 +16399,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V163" t="inlineStr">
+        <is>
+          <t>Journalism and Public Policy</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -15686,6 +16501,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V164" t="inlineStr">
+        <is>
+          <t>Journalism and Public Policy</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -15783,6 +16603,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V165" t="inlineStr">
+        <is>
+          <t>Journalism and Public Policy</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -15880,6 +16705,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V166" t="inlineStr">
+        <is>
+          <t>Journalism and Public Policy</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -15977,6 +16807,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V167" t="inlineStr">
+        <is>
+          <t>Natural Language and Multimodal Interaction</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -16074,6 +16909,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V168" t="inlineStr">
+        <is>
+          <t>Natural Language and Multimodal Interaction</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -16171,6 +17011,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V169" t="inlineStr">
+        <is>
+          <t>Natural Language and Multimodal Interaction</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -16268,6 +17113,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V170" t="inlineStr">
+        <is>
+          <t>Natural Language and Multimodal Interaction</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -16365,6 +17215,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V171" t="inlineStr">
+        <is>
+          <t>Natural Language and Multimodal Interaction</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -16462,6 +17317,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V172" t="inlineStr">
+        <is>
+          <t>Look, Learn, Language Models</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -16559,6 +17419,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V173" t="inlineStr">
+        <is>
+          <t>Look, Learn, Language Models</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -16656,6 +17521,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V174" t="inlineStr">
+        <is>
+          <t>Look, Learn, Language Models</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -16753,6 +17623,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V175" t="inlineStr">
+        <is>
+          <t>Look, Learn, Language Models</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -16854,6 +17729,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V176" t="inlineStr">
+        <is>
+          <t>Look, Learn, Language Models</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -16951,6 +17831,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V177" t="inlineStr">
+        <is>
+          <t>Biological Data Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -17048,6 +17933,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V178" t="inlineStr">
+        <is>
+          <t>Biological Data Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -17145,6 +18035,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V179" t="inlineStr">
+        <is>
+          <t>Biological Data Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -17242,6 +18137,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V180" t="inlineStr">
+        <is>
+          <t>Biological Data Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -17343,6 +18243,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V181" t="inlineStr">
+        <is>
+          <t>Biological Data Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -17440,6 +18345,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V182" t="inlineStr">
+        <is>
+          <t>Immersive Visualization and Visual Analytics</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -17537,6 +18447,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V183" t="inlineStr">
+        <is>
+          <t>Immersive Visualization and Visual Analytics</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -17634,6 +18549,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V184" t="inlineStr">
+        <is>
+          <t>Immersive Visualization and Visual Analytics</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -17731,6 +18651,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V185" t="inlineStr">
+        <is>
+          <t>Immersive Visualization and Visual Analytics</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -17828,6 +18753,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V186" t="inlineStr">
+        <is>
+          <t>Immersive Visualization and Visual Analytics</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -17925,6 +18855,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V187" t="inlineStr">
+        <is>
+          <t>Machine Learning for Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -18022,6 +18957,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V188" t="inlineStr">
+        <is>
+          <t>Machine Learning for Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -18119,6 +19059,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V189" t="inlineStr">
+        <is>
+          <t>Machine Learning for Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -18216,6 +19161,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V190" t="inlineStr">
+        <is>
+          <t>Machine Learning for Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -18313,6 +19263,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V191" t="inlineStr">
+        <is>
+          <t>Machine Learning for Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -18410,6 +19365,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V192" t="inlineStr">
+        <is>
+          <t>Where the Networks Are</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -18507,6 +19467,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V193" t="inlineStr">
+        <is>
+          <t>Where the Networks Are</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -18604,6 +19569,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V194" t="inlineStr">
+        <is>
+          <t>Where the Networks Are</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -18701,6 +19671,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V195" t="inlineStr">
+        <is>
+          <t>Where the Networks Are</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -18798,6 +19773,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V196" t="inlineStr">
+        <is>
+          <t>Where the Networks Are</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -18895,6 +19875,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V197" t="inlineStr">
+        <is>
+          <t>Visualization Recommendation</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -18992,6 +19977,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V198" t="inlineStr">
+        <is>
+          <t>Visualization Recommendation</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -19089,6 +20079,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V199" t="inlineStr">
+        <is>
+          <t>Visualization Recommendation</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -19186,6 +20181,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V200" t="inlineStr">
+        <is>
+          <t>Visualization Recommendation</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -19287,6 +20287,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V201" t="inlineStr">
+        <is>
+          <t>Visualization Recommendation</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -19384,6 +20389,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V202" t="inlineStr">
+        <is>
+          <t>Judgment and Decision-making</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -19481,6 +20491,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V203" t="inlineStr">
+        <is>
+          <t>Judgment and Decision-making</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -19578,6 +20593,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V204" t="inlineStr">
+        <is>
+          <t>Judgment and Decision-making</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -19675,6 +20695,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V205" t="inlineStr">
+        <is>
+          <t>Judgment and Decision-making</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -19772,6 +20797,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V206" t="inlineStr">
+        <is>
+          <t>Judgment and Decision-making</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -19869,6 +20899,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V207" t="inlineStr">
+        <is>
+          <t>Model-checking and Validation</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -19966,6 +21001,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V208" t="inlineStr">
+        <is>
+          <t>Model-checking and Validation</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -20063,6 +21103,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V209" t="inlineStr">
+        <is>
+          <t>Model-checking and Validation</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -20160,6 +21205,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V210" t="inlineStr">
+        <is>
+          <t>Model-checking and Validation</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -20257,6 +21307,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V211" t="inlineStr">
+        <is>
+          <t>Model-checking and Validation</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -20354,6 +21409,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V212" t="inlineStr">
+        <is>
+          <t>Time and Sequences</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -20451,6 +21511,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V213" t="inlineStr">
+        <is>
+          <t>Time and Sequences</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -20548,6 +21613,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V214" t="inlineStr">
+        <is>
+          <t>Time and Sequences</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -20645,6 +21715,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V215" t="inlineStr">
+        <is>
+          <t>Time and Sequences</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -20742,6 +21817,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V216" t="inlineStr">
+        <is>
+          <t>Time and Sequences</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -20839,6 +21919,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V217" t="inlineStr">
+        <is>
+          <t>Accessibility and Touch</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -20940,6 +22025,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V218" t="inlineStr">
+        <is>
+          <t>Accessibility and Touch</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -21041,6 +22131,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V219" t="inlineStr">
+        <is>
+          <t>Accessibility and Touch</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -21138,6 +22233,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V220" t="inlineStr">
+        <is>
+          <t>Accessibility and Touch</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -21235,6 +22335,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V221" t="inlineStr">
+        <is>
+          <t>Collaboration and Communication</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -21332,6 +22437,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V222" t="inlineStr">
+        <is>
+          <t>Collaboration and Communication</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -21429,6 +22539,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V223" t="inlineStr">
+        <is>
+          <t>Collaboration and Communication</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -21526,6 +22641,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V224" t="inlineStr">
+        <is>
+          <t>Collaboration and Communication</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -21627,6 +22747,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V225" t="inlineStr">
+        <is>
+          <t>Collaboration and Communication</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -21724,6 +22849,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V226" t="inlineStr">
+        <is>
+          <t>Once Upon a Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -21821,6 +22951,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V227" t="inlineStr">
+        <is>
+          <t>Once Upon a Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -21918,6 +23053,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V228" t="inlineStr">
+        <is>
+          <t>Once Upon a Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -22015,6 +23155,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V229" t="inlineStr">
+        <is>
+          <t>Once Upon a Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -22112,6 +23257,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V230" t="inlineStr">
+        <is>
+          <t>Once Upon a Visualization</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -22209,6 +23359,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V231" t="inlineStr">
+        <is>
+          <t>Perception and Cognition</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -22306,6 +23461,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V232" t="inlineStr">
+        <is>
+          <t>Perception and Cognition</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -22403,6 +23563,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V233" t="inlineStr">
+        <is>
+          <t>Perception and Cognition</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -22500,6 +23665,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V234" t="inlineStr">
+        <is>
+          <t>Perception and Cognition</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -22597,6 +23767,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V235" t="inlineStr">
+        <is>
+          <t>Perception and Cognition</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -22694,6 +23869,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V236" t="inlineStr">
+        <is>
+          <t>Of Nodes and Networks</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -22791,6 +23971,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V237" t="inlineStr">
+        <is>
+          <t>Of Nodes and Networks</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -22888,6 +24073,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V238" t="inlineStr">
+        <is>
+          <t>Of Nodes and Networks</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -22985,6 +24175,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V239" t="inlineStr">
+        <is>
+          <t>Of Nodes and Networks</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -23082,6 +24277,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V240" t="inlineStr">
+        <is>
+          <t>Of Nodes and Networks</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -23179,6 +24379,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V241" t="inlineStr">
+        <is>
+          <t>Human and Machine Visualization Literacy</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -23280,6 +24485,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V242" t="inlineStr">
+        <is>
+          <t>Human and Machine Visualization Literacy</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -23377,6 +24587,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V243" t="inlineStr">
+        <is>
+          <t>Human and Machine Visualization Literacy</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -23474,6 +24689,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V244" t="inlineStr">
+        <is>
+          <t>Human and Machine Visualization Literacy</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -23571,6 +24791,11 @@
           <t>Friday (Oct 18)</t>
         </is>
       </c>
+      <c r="V245" t="inlineStr">
+        <is>
+          <t>Human and Machine Visualization Literacy</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -23668,6 +24893,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V246" t="inlineStr">
+        <is>
+          <t>Visualization Design Methods</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -23765,6 +24995,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V247" t="inlineStr">
+        <is>
+          <t>Visualization Design Methods</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -23862,6 +25097,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V248" t="inlineStr">
+        <is>
+          <t>Visualization Design Methods</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -23959,6 +25199,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V249" t="inlineStr">
+        <is>
+          <t>Visualization Design Methods</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -24056,6 +25301,11 @@
           <t>Thursday (Oct 17)</t>
         </is>
       </c>
+      <c r="V250" t="inlineStr">
+        <is>
+          <t>Visualization Design Methods</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -24153,6 +25403,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V251" t="inlineStr">
+        <is>
+          <t>Scripts, Notebooks, and Provenance</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -24250,6 +25505,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V252" t="inlineStr">
+        <is>
+          <t>Scripts, Notebooks, and Provenance</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -24347,6 +25607,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V253" t="inlineStr">
+        <is>
+          <t>Scripts, Notebooks, and Provenance</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -24444,6 +25709,11 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V254" t="inlineStr">
+        <is>
+          <t>Scripts, Notebooks, and Provenance</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -24541,11 +25811,16 @@
           <t>Wednesday (Oct 16)</t>
         </is>
       </c>
+      <c r="V255" t="inlineStr">
+        <is>
+          <t>Scripts, Notebooks, and Provenance</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Visual Design-Sketching and Labeling</t>
+          <t>Visual Design: Sketching and Labeling</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -24636,13 +25911,18 @@
       <c r="U256" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V256" t="inlineStr">
+        <is>
+          <t>Visual Design-Sketching and Labeling</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Visual Design-Sketching and Labeling</t>
+          <t>Visual Design: Sketching and Labeling</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -24733,13 +26013,18 @@
       <c r="U257" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V257" t="inlineStr">
+        <is>
+          <t>Visual Design-Sketching and Labeling</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Visual Design-Sketching and Labeling</t>
+          <t>Visual Design: Sketching and Labeling</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -24830,13 +26115,18 @@
       <c r="U258" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V258" t="inlineStr">
+        <is>
+          <t>Visual Design-Sketching and Labeling</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Visual Design-Sketching and Labeling</t>
+          <t>Visual Design: Sketching and Labeling</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -24927,13 +26217,18 @@
       <c r="U259" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V259" t="inlineStr">
+        <is>
+          <t>Visual Design-Sketching and Labeling</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Visual Design-Sketching and Labeling</t>
+          <t>Visual Design: Sketching and Labeling</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -25024,13 +26319,18 @@
       <c r="U260" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V260" t="inlineStr">
+        <is>
+          <t>Visual Design-Sketching and Labeling</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Virtual-VIS from around the world</t>
+          <t>Virtual: VIS from around the world</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -25121,13 +26421,18 @@
       <c r="U261" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V261" t="inlineStr">
+        <is>
+          <t>Virtual-VIS from around the world</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Virtual-VIS from around the world</t>
+          <t>Virtual: VIS from around the world</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -25218,13 +26523,18 @@
       <c r="U262" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V262" t="inlineStr">
+        <is>
+          <t>Virtual-VIS from around the world</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Virtual-VIS from around the world</t>
+          <t>Virtual: VIS from around the world</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -25315,13 +26625,18 @@
       <c r="U263" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V263" t="inlineStr">
+        <is>
+          <t>Virtual-VIS from around the world</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Virtual-VIS from around the world</t>
+          <t>Virtual: VIS from around the world</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -25412,13 +26727,18 @@
       <c r="U264" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V264" t="inlineStr">
+        <is>
+          <t>Virtual-VIS from around the world</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>Virtual-VIS from around the world</t>
+          <t>Virtual: VIS from around the world</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -25509,13 +26829,18 @@
       <c r="U265" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V265" t="inlineStr">
+        <is>
+          <t>Virtual-VIS from around the world</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Virtual-VIS from around the world</t>
+          <t>Virtual: VIS from around the world</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -25606,13 +26931,18 @@
       <c r="U266" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V266" t="inlineStr">
+        <is>
+          <t>Virtual-VIS from around the world</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>Short Papers- System design</t>
+          <t>Short Papers:  System design</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -25703,13 +27033,18 @@
       <c r="U267" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V267" t="inlineStr">
+        <is>
+          <t>Short Papers- System design</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>Short Papers- System design</t>
+          <t>Short Papers:  System design</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -25800,13 +27135,18 @@
       <c r="U268" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V268" t="inlineStr">
+        <is>
+          <t>Short Papers- System design</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>Short Papers- System design</t>
+          <t>Short Papers:  System design</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -25897,13 +27237,18 @@
       <c r="U269" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V269" t="inlineStr">
+        <is>
+          <t>Short Papers- System design</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>Short Papers- System design</t>
+          <t>Short Papers:  System design</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -25994,13 +27339,18 @@
       <c r="U270" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V270" t="inlineStr">
+        <is>
+          <t>Short Papers- System design</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Short Papers- System design</t>
+          <t>Short Papers:  System design</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -26091,13 +27441,18 @@
       <c r="U271" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V271" t="inlineStr">
+        <is>
+          <t>Short Papers- System design</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Short Papers- System design</t>
+          <t>Short Papers:  System design</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -26192,13 +27547,18 @@
       <c r="U272" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V272" t="inlineStr">
+        <is>
+          <t>Short Papers- System design</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>Short Papers- System design</t>
+          <t>Short Papers:  System design</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -26289,13 +27649,18 @@
       <c r="U273" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V273" t="inlineStr">
+        <is>
+          <t>Short Papers- System design</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Short Papers-Analytics and Applications</t>
+          <t>Short Papers: Analytics and Applications</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -26386,13 +27751,18 @@
       <c r="U274" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V274" t="inlineStr">
+        <is>
+          <t>Short Papers-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>Short Papers-Analytics and Applications</t>
+          <t>Short Papers: Analytics and Applications</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -26483,13 +27853,18 @@
       <c r="U275" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V275" t="inlineStr">
+        <is>
+          <t>Short Papers-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>Short Papers-Analytics and Applications</t>
+          <t>Short Papers: Analytics and Applications</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -26580,13 +27955,18 @@
       <c r="U276" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V276" t="inlineStr">
+        <is>
+          <t>Short Papers-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>Short Papers-Analytics and Applications</t>
+          <t>Short Papers: Analytics and Applications</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -26677,13 +28057,18 @@
       <c r="U277" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V277" t="inlineStr">
+        <is>
+          <t>Short Papers-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>Short Papers-Analytics and Applications</t>
+          <t>Short Papers: Analytics and Applications</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -26774,13 +28159,18 @@
       <c r="U278" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V278" t="inlineStr">
+        <is>
+          <t>Short Papers-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>Short Papers-Analytics and Applications</t>
+          <t>Short Papers: Analytics and Applications</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -26871,13 +28261,18 @@
       <c r="U279" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V279" t="inlineStr">
+        <is>
+          <t>Short Papers-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>Short Papers-Analytics and Applications</t>
+          <t>Short Papers: Analytics and Applications</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -26968,13 +28363,18 @@
       <c r="U280" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V280" t="inlineStr">
+        <is>
+          <t>Short Papers-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>Short Papers-AI and LLM</t>
+          <t>Short Papers: AI and LLM</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -27065,13 +28465,18 @@
       <c r="U281" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V281" t="inlineStr">
+        <is>
+          <t>Short Papers-AI and LLM</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>Short Papers-AI and LLM</t>
+          <t>Short Papers: AI and LLM</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -27162,13 +28567,18 @@
       <c r="U282" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V282" t="inlineStr">
+        <is>
+          <t>Short Papers-AI and LLM</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>Short Papers-AI and LLM</t>
+          <t>Short Papers: AI and LLM</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -27259,13 +28669,18 @@
       <c r="U283" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V283" t="inlineStr">
+        <is>
+          <t>Short Papers-AI and LLM</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>Short Papers-AI and LLM</t>
+          <t>Short Papers: AI and LLM</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -27356,13 +28771,18 @@
       <c r="U284" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V284" t="inlineStr">
+        <is>
+          <t>Short Papers-AI and LLM</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>Short Papers-AI and LLM</t>
+          <t>Short Papers: AI and LLM</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -27453,13 +28873,18 @@
       <c r="U285" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V285" t="inlineStr">
+        <is>
+          <t>Short Papers-AI and LLM</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>Short Papers-AI and LLM</t>
+          <t>Short Papers: AI and LLM</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -27550,13 +28975,18 @@
       <c r="U286" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V286" t="inlineStr">
+        <is>
+          <t>Short Papers-AI and LLM</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>Short Papers-AI and LLM</t>
+          <t>Short Papers: AI and LLM</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -27647,13 +29077,18 @@
       <c r="U287" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V287" t="inlineStr">
+        <is>
+          <t>Short Papers-AI and LLM</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
+          <t>Short Papers: Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -27744,13 +29179,18 @@
       <c r="U288" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V288" t="inlineStr">
+        <is>
+          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
+          <t>Short Papers: Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -27841,13 +29281,18 @@
       <c r="U289" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V289" t="inlineStr">
+        <is>
+          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
+          <t>Short Papers: Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -27938,13 +29383,18 @@
       <c r="U290" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V290" t="inlineStr">
+        <is>
+          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
+          <t>Short Papers: Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -28035,13 +29485,18 @@
       <c r="U291" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V291" t="inlineStr">
+        <is>
+          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
+          <t>Short Papers: Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -28132,13 +29587,18 @@
       <c r="U292" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V292" t="inlineStr">
+        <is>
+          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
+          <t>Short Papers: Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -28229,13 +29689,18 @@
       <c r="U293" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V293" t="inlineStr">
+        <is>
+          <t>Short Papers-Graph, Hierarchy and Multidimensional</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>Short Papers-Scientific and Immersive Visualization</t>
+          <t>Short Papers: Scientific and Immersive Visualization</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -28330,13 +29795,18 @@
       <c r="U294" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V294" t="inlineStr">
+        <is>
+          <t>Short Papers-Scientific and Immersive Visualization</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>Short Papers-Scientific and Immersive Visualization</t>
+          <t>Short Papers: Scientific and Immersive Visualization</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -28427,13 +29897,18 @@
       <c r="U295" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V295" t="inlineStr">
+        <is>
+          <t>Short Papers-Scientific and Immersive Visualization</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>Short Papers-Scientific and Immersive Visualization</t>
+          <t>Short Papers: Scientific and Immersive Visualization</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -28524,13 +29999,18 @@
       <c r="U296" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V296" t="inlineStr">
+        <is>
+          <t>Short Papers-Scientific and Immersive Visualization</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>Short Papers-Scientific and Immersive Visualization</t>
+          <t>Short Papers: Scientific and Immersive Visualization</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -28621,13 +30101,18 @@
       <c r="U297" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V297" t="inlineStr">
+        <is>
+          <t>Short Papers-Scientific and Immersive Visualization</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>Short Papers-Scientific and Immersive Visualization</t>
+          <t>Short Papers: Scientific and Immersive Visualization</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -28718,13 +30203,18 @@
       <c r="U298" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V298" t="inlineStr">
+        <is>
+          <t>Short Papers-Scientific and Immersive Visualization</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>Short Papers-Scientific and Immersive Visualization</t>
+          <t>Short Papers: Scientific and Immersive Visualization</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
@@ -28815,13 +30305,18 @@
       <c r="U299" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V299" t="inlineStr">
+        <is>
+          <t>Short Papers-Scientific and Immersive Visualization</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>Short Papers-Scientific and Immersive Visualization</t>
+          <t>Short Papers: Scientific and Immersive Visualization</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -28912,13 +30407,18 @@
       <c r="U300" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V300" t="inlineStr">
+        <is>
+          <t>Short Papers-Scientific and Immersive Visualization</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>Short Papers-Perception and Representation</t>
+          <t>Short Papers: Perception and Representation</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -29009,13 +30509,18 @@
       <c r="U301" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V301" t="inlineStr">
+        <is>
+          <t>Short Papers-Perception and Representation</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>Short Papers-Perception and Representation</t>
+          <t>Short Papers: Perception and Representation</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -29106,13 +30611,18 @@
       <c r="U302" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V302" t="inlineStr">
+        <is>
+          <t>Short Papers-Perception and Representation</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>Short Papers-Perception and Representation</t>
+          <t>Short Papers: Perception and Representation</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -29203,13 +30713,18 @@
       <c r="U303" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V303" t="inlineStr">
+        <is>
+          <t>Short Papers-Perception and Representation</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>Short Papers-Perception and Representation</t>
+          <t>Short Papers: Perception and Representation</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -29300,13 +30815,18 @@
       <c r="U304" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V304" t="inlineStr">
+        <is>
+          <t>Short Papers-Perception and Representation</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>Short Papers-Perception and Representation</t>
+          <t>Short Papers: Perception and Representation</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
@@ -29397,13 +30917,18 @@
       <c r="U305" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V305" t="inlineStr">
+        <is>
+          <t>Short Papers-Perception and Representation</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>Short Papers-Perception and Representation</t>
+          <t>Short Papers: Perception and Representation</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -29494,13 +31019,18 @@
       <c r="U306" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V306" t="inlineStr">
+        <is>
+          <t>Short Papers-Perception and Representation</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>Short Papers-Perception and Representation</t>
+          <t>Short Papers: Perception and Representation</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -29591,13 +31121,18 @@
       <c r="U307" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V307" t="inlineStr">
+        <is>
+          <t>Short Papers-Perception and Representation</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>Short Papers-Text and Multimedia</t>
+          <t>Short Papers: Text and Multimedia</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -29688,13 +31223,18 @@
       <c r="U308" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V308" t="inlineStr">
+        <is>
+          <t>Short Papers-Text and Multimedia</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>Short Papers-Text and Multimedia</t>
+          <t>Short Papers: Text and Multimedia</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -29785,13 +31325,18 @@
       <c r="U309" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V309" t="inlineStr">
+        <is>
+          <t>Short Papers-Text and Multimedia</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>Short Papers-Text and Multimedia</t>
+          <t>Short Papers: Text and Multimedia</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -29882,13 +31427,18 @@
       <c r="U310" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V310" t="inlineStr">
+        <is>
+          <t>Short Papers-Text and Multimedia</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>Short Papers-Text and Multimedia</t>
+          <t>Short Papers: Text and Multimedia</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -29979,13 +31529,18 @@
       <c r="U311" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V311" t="inlineStr">
+        <is>
+          <t>Short Papers-Text and Multimedia</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>Short Papers-Text and Multimedia</t>
+          <t>Short Papers: Text and Multimedia</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
@@ -30076,13 +31631,18 @@
       <c r="U312" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V312" t="inlineStr">
+        <is>
+          <t>Short Papers-Text and Multimedia</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>Short Papers-Text and Multimedia</t>
+          <t>Short Papers: Text and Multimedia</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -30173,13 +31733,18 @@
       <c r="U313" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V313" t="inlineStr">
+        <is>
+          <t>Short Papers-Text and Multimedia</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>Short Papers-Text and Multimedia</t>
+          <t>Short Papers: Text and Multimedia</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
@@ -30270,13 +31835,18 @@
       <c r="U314" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V314" t="inlineStr">
+        <is>
+          <t>Short Papers-Text and Multimedia</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>CG&amp;A-Analytics and Applications</t>
+          <t>CG&amp;A: Analytics and Applications</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -30367,13 +31937,18 @@
       <c r="U315" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V315" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>CG&amp;A-Analytics and Applications</t>
+          <t>CG&amp;A: Analytics and Applications</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -30464,13 +32039,18 @@
       <c r="U316" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V316" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>CG&amp;A-Analytics and Applications</t>
+          <t>CG&amp;A: Analytics and Applications</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
@@ -30561,13 +32141,18 @@
       <c r="U317" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V317" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>CG&amp;A-Analytics and Applications</t>
+          <t>CG&amp;A: Analytics and Applications</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -30658,13 +32243,18 @@
       <c r="U318" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V318" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>CG&amp;A-Analytics and Applications</t>
+          <t>CG&amp;A: Analytics and Applications</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -30755,13 +32345,18 @@
       <c r="U319" t="inlineStr">
         <is>
           <t>Wednesday (Oct 16)</t>
+        </is>
+      </c>
+      <c r="V319" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Analytics and Applications</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
+          <t>CG&amp;A: Systems, Theory, and Evaluations</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -30852,13 +32447,18 @@
       <c r="U320" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V320" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
+          <t>CG&amp;A: Systems, Theory, and Evaluations</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -30949,13 +32549,18 @@
       <c r="U321" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V321" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
+          <t>CG&amp;A: Systems, Theory, and Evaluations</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -31046,13 +32651,18 @@
       <c r="U322" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V322" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
+          <t>CG&amp;A: Systems, Theory, and Evaluations</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -31143,13 +32753,18 @@
       <c r="U323" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V323" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
+          <t>CG&amp;A: Systems, Theory, and Evaluations</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -31240,6 +32855,11 @@
       <c r="U324" t="inlineStr">
         <is>
           <t>Thursday (Oct 17)</t>
+        </is>
+      </c>
+      <c r="V324" t="inlineStr">
+        <is>
+          <t>CG&amp;A-Systems, Theory, and Evaluations</t>
         </is>
       </c>
     </row>

</xml_diff>